<commit_message>
Fixed timeout bug with invalid block propositions
</commit_message>
<xml_diff>
--- a/Storage/B_visualization_timeout.xlsx
+++ b/Storage/B_visualization_timeout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spaul/Documents/BlockchainTest/Storage/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A49FD13-0832-2141-A1EB-B3A30AA85937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DBF97F-EF75-0541-A16B-C0A01A3F6178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{48C39ACA-1444-E34E-8EEF-7B627AA91503}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{48C39ACA-1444-E34E-8EEF-7B627AA91503}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5758,6 +5758,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Block Index</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5776,7 +5831,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5823,6 +5878,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>UtilityToken</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Balance</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -6838,7 +6953,7 @@
   <dimension ref="A1:U38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>